<commit_message>
Update WBS_Levi‘s CMS System SI_(CN-HK)_20190814.xlsx
根据8/26截止日期。管理3天 导入2天的工时
</commit_message>
<xml_diff>
--- a/2019/香港店/99 项目管理/WBS_Levi‘s CMS System SI_(CN-HK)_20190814.xlsx
+++ b/2019/香港店/99 项目管理/WBS_Levi‘s CMS System SI_(CN-HK)_20190814.xlsx
@@ -939,10 +939,6 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>CMS系统导入</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
     <t>项目测试</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
@@ -1187,10 +1183,6 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>JP-TKY-Sibuya专用账号登记</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
     <t>导入计划编制</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
@@ -1347,18 +1339,6 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>LED设备内容审核</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
-    <t>各楼层拼接屏设备内容审核</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
-    <t>各楼层拼接屏设备内容编制</t>
-    <phoneticPr fontId="24" type="noConversion"/>
-  </si>
-  <si>
     <t>设备长时间运行测试</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
@@ -1451,11 +1431,15 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>LED切屏方案</t>
+    <t>安装线路设计</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>安装线路设计</t>
+    <t>香港现场勘察</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED切屏方案</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
@@ -1463,7 +1447,23 @@
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
   <si>
-    <t>香港现场勘察</t>
+    <t>LED设备内容审核</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>各楼层拼接屏设备内容编制</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>各楼层拼接屏设备内容审核</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMS系统导入</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>专用账号登记</t>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
 </sst>
@@ -3781,6 +3781,15 @@
     <xf numFmtId="0" fontId="46" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3957,15 +3966,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -3978,7 +3978,14 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="未定義" xfId="7"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5160,10 +5167,10 @@
   </sheetPr>
   <dimension ref="A1:BG127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -5185,32 +5192,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="19.5" customHeight="1" thickTop="1">
-      <c r="A1" s="304" t="s">
-        <v>294</v>
-      </c>
-      <c r="B1" s="305"/>
-      <c r="C1" s="305"/>
-      <c r="D1" s="305"/>
-      <c r="E1" s="305"/>
-      <c r="F1" s="305"/>
-      <c r="G1" s="305"/>
-      <c r="H1" s="305"/>
+      <c r="A1" s="307" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="308"/>
+      <c r="C1" s="308"/>
+      <c r="D1" s="308"/>
+      <c r="E1" s="308"/>
+      <c r="F1" s="308"/>
+      <c r="G1" s="308"/>
+      <c r="H1" s="308"/>
       <c r="I1" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="329" t="s">
+      <c r="J1" s="332" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="330"/>
+      <c r="K1" s="333"/>
       <c r="L1" s="118" t="s">
         <v>170</v>
       </c>
-      <c r="M1" s="329" t="s">
+      <c r="M1" s="332" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="331"/>
-      <c r="O1" s="325"/>
-      <c r="P1" s="326"/>
+      <c r="N1" s="334"/>
+      <c r="O1" s="328"/>
+      <c r="P1" s="329"/>
       <c r="Q1" s="119"/>
       <c r="R1" s="119"/>
       <c r="S1" s="119"/>
@@ -5220,30 +5227,30 @@
       <c r="W1" s="119"/>
     </row>
     <row r="2" spans="1:59" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A2" s="306"/>
-      <c r="B2" s="307"/>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="G2" s="307"/>
-      <c r="H2" s="307"/>
+      <c r="A2" s="309"/>
+      <c r="B2" s="310"/>
+      <c r="C2" s="310"/>
+      <c r="D2" s="310"/>
+      <c r="E2" s="310"/>
+      <c r="F2" s="310"/>
+      <c r="G2" s="310"/>
+      <c r="H2" s="310"/>
       <c r="I2" s="120" t="s">
-        <v>226</v>
-      </c>
-      <c r="J2" s="332">
+        <v>225</v>
+      </c>
+      <c r="J2" s="335">
         <v>43691</v>
       </c>
-      <c r="K2" s="333"/>
+      <c r="K2" s="336"/>
       <c r="L2" s="121" t="s">
-        <v>219</v>
-      </c>
-      <c r="M2" s="332">
-        <v>43691</v>
-      </c>
-      <c r="N2" s="334"/>
-      <c r="O2" s="327"/>
-      <c r="P2" s="328"/>
+        <v>218</v>
+      </c>
+      <c r="M2" s="335">
+        <v>43692</v>
+      </c>
+      <c r="N2" s="337"/>
+      <c r="O2" s="330"/>
+      <c r="P2" s="331"/>
       <c r="Q2" s="119"/>
       <c r="R2" s="119"/>
       <c r="S2" s="119"/>
@@ -5278,36 +5285,36 @@
       <c r="W3" s="122"/>
     </row>
     <row r="4" spans="1:59" ht="23.25" customHeight="1">
-      <c r="A4" s="312" t="s">
+      <c r="A4" s="315" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="313"/>
-      <c r="C4" s="313"/>
-      <c r="D4" s="314"/>
-      <c r="E4" s="314"/>
-      <c r="F4" s="317" t="s">
+      <c r="B4" s="316"/>
+      <c r="C4" s="316"/>
+      <c r="D4" s="317"/>
+      <c r="E4" s="317"/>
+      <c r="F4" s="320" t="s">
         <v>171</v>
       </c>
-      <c r="G4" s="319" t="s">
-        <v>185</v>
-      </c>
-      <c r="H4" s="321" t="s">
+      <c r="G4" s="322" t="s">
+        <v>184</v>
+      </c>
+      <c r="H4" s="324" t="s">
         <v>164</v>
       </c>
-      <c r="I4" s="322" t="s">
+      <c r="I4" s="325" t="s">
         <v>165</v>
       </c>
-      <c r="J4" s="323"/>
-      <c r="K4" s="324"/>
-      <c r="L4" s="322" t="s">
+      <c r="J4" s="326"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="325" t="s">
         <v>166</v>
       </c>
-      <c r="M4" s="323"/>
-      <c r="N4" s="324"/>
-      <c r="O4" s="308" t="s">
+      <c r="M4" s="326"/>
+      <c r="N4" s="327"/>
+      <c r="O4" s="311" t="s">
         <v>174</v>
       </c>
-      <c r="P4" s="310" t="s">
+      <c r="P4" s="313" t="s">
         <v>168</v>
       </c>
       <c r="Q4" s="122"/>
@@ -5458,14 +5465,14 @@
       </c>
     </row>
     <row r="5" spans="1:59" ht="41.25" thickBot="1">
-      <c r="A5" s="315"/>
-      <c r="B5" s="316"/>
-      <c r="C5" s="316"/>
-      <c r="D5" s="316"/>
-      <c r="E5" s="316"/>
-      <c r="F5" s="318"/>
-      <c r="G5" s="320"/>
-      <c r="H5" s="320"/>
+      <c r="A5" s="318"/>
+      <c r="B5" s="319"/>
+      <c r="C5" s="319"/>
+      <c r="D5" s="319"/>
+      <c r="E5" s="319"/>
+      <c r="F5" s="321"/>
+      <c r="G5" s="323"/>
+      <c r="H5" s="323"/>
       <c r="I5" s="152" t="s">
         <v>176</v>
       </c>
@@ -5484,8 +5491,8 @@
       <c r="N5" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="O5" s="309"/>
-      <c r="P5" s="311"/>
+      <c r="O5" s="312"/>
+      <c r="P5" s="314"/>
       <c r="Q5" s="122"/>
       <c r="R5" s="129" t="s">
         <v>158</v>
@@ -5500,109 +5507,109 @@
       <c r="V5" s="122"/>
       <c r="W5" s="122"/>
       <c r="Y5" s="269" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z5" s="270" t="s">
+        <v>270</v>
+      </c>
+      <c r="AA5" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="Z5" s="270" t="s">
+      <c r="AB5" s="270" t="s">
         <v>272</v>
       </c>
-      <c r="AA5" s="270" t="s">
+      <c r="AC5" s="270" t="s">
         <v>273</v>
       </c>
-      <c r="AB5" s="270" t="s">
+      <c r="AD5" s="270" t="s">
         <v>274</v>
       </c>
-      <c r="AC5" s="270" t="s">
+      <c r="AE5" s="270" t="s">
         <v>275</v>
       </c>
-      <c r="AD5" s="270" t="s">
-        <v>276</v>
-      </c>
-      <c r="AE5" s="270" t="s">
-        <v>277</v>
-      </c>
       <c r="AF5" s="270" t="s">
+        <v>269</v>
+      </c>
+      <c r="AG5" s="270" t="s">
+        <v>270</v>
+      </c>
+      <c r="AH5" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="AG5" s="270" t="s">
+      <c r="AI5" s="270" t="s">
         <v>272</v>
       </c>
-      <c r="AH5" s="270" t="s">
+      <c r="AJ5" s="270" t="s">
         <v>273</v>
       </c>
-      <c r="AI5" s="270" t="s">
+      <c r="AK5" s="270" t="s">
         <v>274</v>
       </c>
-      <c r="AJ5" s="270" t="s">
+      <c r="AL5" s="270" t="s">
         <v>275</v>
       </c>
-      <c r="AK5" s="270" t="s">
-        <v>276</v>
-      </c>
-      <c r="AL5" s="270" t="s">
-        <v>277</v>
-      </c>
       <c r="AM5" s="270" t="s">
+        <v>269</v>
+      </c>
+      <c r="AN5" s="270" t="s">
+        <v>270</v>
+      </c>
+      <c r="AO5" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="AN5" s="270" t="s">
+      <c r="AP5" s="270" t="s">
         <v>272</v>
       </c>
-      <c r="AO5" s="270" t="s">
+      <c r="AQ5" s="270" t="s">
         <v>273</v>
       </c>
-      <c r="AP5" s="270" t="s">
+      <c r="AR5" s="270" t="s">
         <v>274</v>
       </c>
-      <c r="AQ5" s="270" t="s">
+      <c r="AS5" s="270" t="s">
         <v>275</v>
       </c>
-      <c r="AR5" s="270" t="s">
-        <v>276</v>
-      </c>
-      <c r="AS5" s="270" t="s">
-        <v>277</v>
-      </c>
       <c r="AT5" s="270" t="s">
+        <v>269</v>
+      </c>
+      <c r="AU5" s="270" t="s">
+        <v>270</v>
+      </c>
+      <c r="AV5" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="AU5" s="270" t="s">
+      <c r="AW5" s="270" t="s">
         <v>272</v>
       </c>
-      <c r="AV5" s="270" t="s">
+      <c r="AX5" s="270" t="s">
         <v>273</v>
       </c>
-      <c r="AW5" s="270" t="s">
+      <c r="AY5" s="270" t="s">
         <v>274</v>
       </c>
-      <c r="AX5" s="270" t="s">
+      <c r="AZ5" s="270" t="s">
         <v>275</v>
       </c>
-      <c r="AY5" s="270" t="s">
-        <v>276</v>
-      </c>
-      <c r="AZ5" s="270" t="s">
-        <v>277</v>
-      </c>
       <c r="BA5" s="270" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB5" s="270" t="s">
+        <v>270</v>
+      </c>
+      <c r="BC5" s="270" t="s">
         <v>271</v>
       </c>
-      <c r="BB5" s="270" t="s">
+      <c r="BD5" s="270" t="s">
         <v>272</v>
       </c>
-      <c r="BC5" s="270" t="s">
+      <c r="BE5" s="270" t="s">
         <v>273</v>
       </c>
-      <c r="BD5" s="270" t="s">
+      <c r="BF5" s="270" t="s">
         <v>274</v>
       </c>
-      <c r="BE5" s="270" t="s">
+      <c r="BG5" s="271" t="s">
         <v>275</v>
-      </c>
-      <c r="BF5" s="270" t="s">
-        <v>276</v>
-      </c>
-      <c r="BG5" s="271" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:59" ht="17.25">
@@ -5794,13 +5801,13 @@
       <c r="D7" s="163"/>
       <c r="E7" s="164"/>
       <c r="F7" s="212" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G7" s="231" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H7" s="223" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I7" s="166"/>
       <c r="J7" s="166"/>
@@ -5810,7 +5817,7 @@
       <c r="N7" s="168"/>
       <c r="O7" s="169"/>
       <c r="P7" s="170" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q7" s="130"/>
       <c r="R7" s="131" t="str">
@@ -5980,18 +5987,26 @@
       <c r="D8" s="163"/>
       <c r="E8" s="164"/>
       <c r="F8" s="212" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G8" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H8" s="223" t="s">
-        <v>219</v>
-      </c>
-      <c r="I8" s="166"/>
-      <c r="J8" s="166"/>
-      <c r="K8" s="167"/>
-      <c r="L8" s="166"/>
+        <v>218</v>
+      </c>
+      <c r="I8" s="166">
+        <v>43678</v>
+      </c>
+      <c r="J8" s="166">
+        <v>43703</v>
+      </c>
+      <c r="K8" s="167">
+        <v>8</v>
+      </c>
+      <c r="L8" s="166">
+        <v>43678</v>
+      </c>
       <c r="M8" s="166"/>
       <c r="N8" s="168"/>
       <c r="O8" s="169">
@@ -5999,17 +6014,17 @@
       </c>
       <c r="P8" s="170"/>
       <c r="Q8" s="130"/>
-      <c r="R8" s="131" t="str">
+      <c r="R8" s="131">
         <f>IF($J8="","",IF($J8&lt;=$L$2,$K8,IF($I8&lt;=$L$2,NETWORKDAYS($I8,$L$2,holiday!$C$3:$C$10)/NETWORKDAYS($I8,$J8,holiday!$C$3:$C$10)*$K8,0)))</f>
-        <v/>
-      </c>
-      <c r="S8" s="131" t="str">
+        <v>8</v>
+      </c>
+      <c r="S8" s="131">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="T8" s="131" t="str">
+        <v>2.4</v>
+      </c>
+      <c r="T8" s="131">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2.4</v>
       </c>
       <c r="U8" s="132"/>
       <c r="V8" s="130"/>
@@ -6166,18 +6181,26 @@
       <c r="D9" s="163"/>
       <c r="E9" s="164"/>
       <c r="F9" s="212" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G9" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H9" s="223" t="s">
-        <v>219</v>
-      </c>
-      <c r="I9" s="166"/>
-      <c r="J9" s="166"/>
-      <c r="K9" s="167"/>
-      <c r="L9" s="166"/>
+        <v>218</v>
+      </c>
+      <c r="I9" s="166">
+        <v>43678</v>
+      </c>
+      <c r="J9" s="166">
+        <v>43703</v>
+      </c>
+      <c r="K9" s="167">
+        <v>18</v>
+      </c>
+      <c r="L9" s="166">
+        <v>43678</v>
+      </c>
       <c r="M9" s="166"/>
       <c r="N9" s="168"/>
       <c r="O9" s="169">
@@ -6185,17 +6208,17 @@
       </c>
       <c r="P9" s="170"/>
       <c r="Q9" s="130"/>
-      <c r="R9" s="131" t="str">
+      <c r="R9" s="131">
         <f>IF($J9="","",IF($J9&lt;=$L$2,$K9,IF($I9&lt;=$L$2,NETWORKDAYS($I9,$L$2,holiday!$C$3:$C$10)/NETWORKDAYS($I9,$J9,holiday!$C$3:$C$10)*$K9,0)))</f>
-        <v/>
-      </c>
-      <c r="S9" s="131" t="str">
+        <v>18</v>
+      </c>
+      <c r="S9" s="131">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="T9" s="131" t="str">
+        <v>4.5</v>
+      </c>
+      <c r="T9" s="131">
         <f t="shared" si="2"/>
-        <v/>
+        <v>4.5</v>
       </c>
       <c r="U9" s="132"/>
       <c r="V9" s="130"/>
@@ -6352,13 +6375,13 @@
       <c r="D10" s="204"/>
       <c r="E10" s="205"/>
       <c r="F10" s="266" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G10" s="267" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H10" s="268" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I10" s="207"/>
       <c r="J10" s="207"/>
@@ -6368,7 +6391,7 @@
       <c r="N10" s="209"/>
       <c r="O10" s="210"/>
       <c r="P10" s="211" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q10" s="130"/>
       <c r="R10" s="131" t="str">
@@ -6538,13 +6561,13 @@
       <c r="D11" s="204"/>
       <c r="E11" s="205"/>
       <c r="F11" s="266" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G11" s="267" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H11" s="268" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I11" s="207"/>
       <c r="J11" s="207"/>
@@ -6554,7 +6577,7 @@
       <c r="N11" s="209"/>
       <c r="O11" s="210"/>
       <c r="P11" s="211" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q11" s="130"/>
       <c r="R11" s="131" t="str">
@@ -6724,13 +6747,13 @@
       <c r="D12" s="204"/>
       <c r="E12" s="205"/>
       <c r="F12" s="266" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G12" s="267" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H12" s="268" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I12" s="207"/>
       <c r="J12" s="207"/>
@@ -6740,7 +6763,7 @@
       <c r="N12" s="209"/>
       <c r="O12" s="210"/>
       <c r="P12" s="211" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q12" s="130"/>
       <c r="R12" s="131" t="str">
@@ -7266,7 +7289,7 @@
       <c r="D15" s="255"/>
       <c r="E15" s="256"/>
       <c r="F15" s="265" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G15" s="257"/>
       <c r="H15" s="258"/>
@@ -7448,10 +7471,10 @@
       <c r="D16" s="163"/>
       <c r="E16" s="164"/>
       <c r="F16" s="219" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G16" s="231" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H16" s="232"/>
       <c r="I16" s="166"/>
@@ -7464,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q16" s="130"/>
       <c r="R16" s="131" t="str">
@@ -7636,10 +7659,10 @@
       <c r="D17" s="163"/>
       <c r="E17" s="164"/>
       <c r="F17" s="233" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G17" s="231" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H17" s="232"/>
       <c r="I17" s="166"/>
@@ -7652,7 +7675,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="286" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="Q17" s="130"/>
       <c r="R17" s="131" t="str">
@@ -7824,13 +7847,13 @@
       <c r="D18" s="163"/>
       <c r="E18" s="164"/>
       <c r="F18" s="233" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G18" s="231" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H18" s="223" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I18" s="166"/>
       <c r="J18" s="166"/>
@@ -7842,7 +7865,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="286" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="Q18" s="130"/>
       <c r="R18" s="131" t="str">
@@ -8014,10 +8037,10 @@
       <c r="D19" s="163"/>
       <c r="E19" s="164"/>
       <c r="F19" s="233" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G19" s="231" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H19" s="232"/>
       <c r="I19" s="166"/>
@@ -8030,7 +8053,7 @@
         <v>1</v>
       </c>
       <c r="P19" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q19" s="130"/>
       <c r="R19" s="131" t="str">
@@ -8202,13 +8225,13 @@
       <c r="D20" s="163"/>
       <c r="E20" s="164"/>
       <c r="F20" s="233" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G20" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H20" s="232" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I20" s="166"/>
       <c r="J20" s="166"/>
@@ -8220,7 +8243,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q20" s="130"/>
       <c r="R20" s="131" t="str">
@@ -8380,25 +8403,25 @@
       </c>
     </row>
     <row r="21" spans="1:59" ht="17.25">
-      <c r="A21" s="360">
+      <c r="A21" s="301">
         <v>1</v>
       </c>
-      <c r="B21" s="361">
+      <c r="B21" s="302">
         <v>1</v>
       </c>
-      <c r="C21" s="361">
+      <c r="C21" s="302">
         <v>7</v>
       </c>
-      <c r="D21" s="361"/>
-      <c r="E21" s="362"/>
+      <c r="D21" s="302"/>
+      <c r="E21" s="303"/>
       <c r="F21" s="233" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G21" s="231" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H21" s="232" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I21" s="166"/>
       <c r="J21" s="166"/>
@@ -8410,7 +8433,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q21" s="130"/>
       <c r="R21" s="131" t="str">
@@ -8760,7 +8783,7 @@
       <c r="D23" s="255"/>
       <c r="E23" s="256"/>
       <c r="F23" s="265" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G23" s="257"/>
       <c r="H23" s="258"/>
@@ -8942,10 +8965,10 @@
       <c r="D24" s="163"/>
       <c r="E24" s="164"/>
       <c r="F24" s="233" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G24" s="231" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H24" s="223"/>
       <c r="I24" s="166"/>
@@ -8958,7 +8981,7 @@
         <v>1</v>
       </c>
       <c r="P24" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q24" s="130"/>
       <c r="R24" s="131" t="str">
@@ -9130,13 +9153,13 @@
       <c r="D25" s="163"/>
       <c r="E25" s="164"/>
       <c r="F25" s="219" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G25" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H25" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I25" s="166"/>
       <c r="J25" s="166"/>
@@ -9148,7 +9171,7 @@
         <v>1</v>
       </c>
       <c r="P25" s="234" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="Q25" s="130"/>
       <c r="R25" s="131" t="str">
@@ -9320,13 +9343,13 @@
       <c r="D26" s="163"/>
       <c r="E26" s="164"/>
       <c r="F26" s="233" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G26" s="231" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H26" s="223" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I26" s="166"/>
       <c r="J26" s="166"/>
@@ -9338,7 +9361,7 @@
         <v>1</v>
       </c>
       <c r="P26" s="286" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="Q26" s="130"/>
       <c r="R26" s="131" t="str">
@@ -9510,10 +9533,10 @@
       <c r="D27" s="163"/>
       <c r="E27" s="164"/>
       <c r="F27" s="219" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G27" s="231" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H27" s="232"/>
       <c r="I27" s="166"/>
@@ -9526,7 +9549,7 @@
         <v>1</v>
       </c>
       <c r="P27" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q27" s="130"/>
       <c r="R27" s="131" t="str">
@@ -9698,13 +9721,13 @@
       <c r="D28" s="163"/>
       <c r="E28" s="164"/>
       <c r="F28" s="233" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G28" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H28" s="232" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I28" s="166"/>
       <c r="J28" s="166"/>
@@ -9716,7 +9739,7 @@
         <v>0.75</v>
       </c>
       <c r="P28" s="234" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="Q28" s="130"/>
       <c r="R28" s="131" t="str">
@@ -9888,13 +9911,13 @@
       <c r="D29" s="163"/>
       <c r="E29" s="164"/>
       <c r="F29" s="233" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G29" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H29" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I29" s="166"/>
       <c r="J29" s="166"/>
@@ -9906,7 +9929,7 @@
         <v>0.75</v>
       </c>
       <c r="P29" s="286" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="Q29" s="130"/>
       <c r="R29" s="131" t="str">
@@ -10078,13 +10101,13 @@
       <c r="D30" s="163"/>
       <c r="E30" s="164"/>
       <c r="F30" s="233" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G30" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H30" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I30" s="166"/>
       <c r="J30" s="166"/>
@@ -10094,7 +10117,7 @@
       <c r="N30" s="168"/>
       <c r="O30" s="169"/>
       <c r="P30" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q30" s="130"/>
       <c r="R30" s="131" t="str">
@@ -10266,13 +10289,13 @@
       <c r="D31" s="163"/>
       <c r="E31" s="164"/>
       <c r="F31" s="233" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G31" s="222" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H31" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I31" s="166"/>
       <c r="J31" s="166"/>
@@ -10282,7 +10305,7 @@
       <c r="N31" s="168"/>
       <c r="O31" s="169"/>
       <c r="P31" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q31" s="130"/>
       <c r="R31" s="131" t="str">
@@ -10527,7 +10550,7 @@
       <c r="D33" s="255"/>
       <c r="E33" s="256"/>
       <c r="F33" s="265" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G33" s="257"/>
       <c r="H33" s="258"/>
@@ -10709,10 +10732,10 @@
       <c r="D34" s="273"/>
       <c r="E34" s="274"/>
       <c r="F34" s="275" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G34" s="279" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H34" s="277"/>
       <c r="I34" s="278"/>
@@ -10893,13 +10916,13 @@
       <c r="D35" s="273"/>
       <c r="E35" s="274"/>
       <c r="F35" s="275" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G35" s="279" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H35" s="277" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I35" s="278"/>
       <c r="J35" s="278"/>
@@ -11079,13 +11102,13 @@
       <c r="D36" s="273"/>
       <c r="E36" s="274"/>
       <c r="F36" s="280" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G36" s="276" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H36" s="277" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I36" s="278"/>
       <c r="J36" s="278"/>
@@ -11265,13 +11288,13 @@
       <c r="D37" s="273"/>
       <c r="E37" s="274"/>
       <c r="F37" s="275" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G37" s="276" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H37" s="277" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I37" s="278"/>
       <c r="J37" s="278"/>
@@ -11451,13 +11474,13 @@
       <c r="D38" s="273"/>
       <c r="E38" s="274"/>
       <c r="F38" s="275" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G38" s="276" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H38" s="277" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I38" s="278"/>
       <c r="J38" s="278"/>
@@ -11888,7 +11911,7 @@
       <c r="D41" s="255"/>
       <c r="E41" s="256"/>
       <c r="F41" s="265" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G41" s="257"/>
       <c r="H41" s="258"/>
@@ -12070,10 +12093,10 @@
       <c r="D42" s="163"/>
       <c r="E42" s="164"/>
       <c r="F42" s="233" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G42" s="231" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H42" s="232"/>
       <c r="I42" s="166"/>
@@ -12254,13 +12277,13 @@
       <c r="D43" s="163"/>
       <c r="E43" s="164"/>
       <c r="F43" s="233" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G43" s="222" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H43" s="223" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I43" s="166"/>
       <c r="J43" s="166"/>
@@ -12440,13 +12463,13 @@
       <c r="D44" s="273"/>
       <c r="E44" s="274"/>
       <c r="F44" s="280" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G44" s="276" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H44" s="277" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I44" s="278"/>
       <c r="J44" s="278"/>
@@ -12456,7 +12479,7 @@
       <c r="N44" s="282"/>
       <c r="O44" s="283"/>
       <c r="P44" s="284" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="Q44" s="130"/>
       <c r="R44" s="131" t="str">
@@ -12806,7 +12829,7 @@
       <c r="D46" s="255"/>
       <c r="E46" s="256"/>
       <c r="F46" s="265" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G46" s="257"/>
       <c r="H46" s="258"/>
@@ -12988,13 +13011,13 @@
       <c r="D47" s="163"/>
       <c r="E47" s="164"/>
       <c r="F47" s="219" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G47" s="222" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H47" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I47" s="166"/>
       <c r="J47" s="166"/>
@@ -13174,13 +13197,13 @@
       <c r="D48" s="163"/>
       <c r="E48" s="164"/>
       <c r="F48" s="219" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G48" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H48" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I48" s="166"/>
       <c r="J48" s="166"/>
@@ -13360,13 +13383,13 @@
       <c r="D49" s="163"/>
       <c r="E49" s="164"/>
       <c r="F49" s="219" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G49" s="222" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H49" s="223" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I49" s="166"/>
       <c r="J49" s="166"/>
@@ -13546,13 +13569,13 @@
       <c r="D50" s="273"/>
       <c r="E50" s="274"/>
       <c r="F50" s="275" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G50" s="276" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H50" s="277" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I50" s="278"/>
       <c r="J50" s="278"/>
@@ -13562,7 +13585,7 @@
       <c r="N50" s="282"/>
       <c r="O50" s="283"/>
       <c r="P50" s="298" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="Q50" s="130"/>
       <c r="R50" s="131" t="str">
@@ -13912,7 +13935,7 @@
       <c r="D52" s="255"/>
       <c r="E52" s="256"/>
       <c r="F52" s="265" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G52" s="257"/>
       <c r="H52" s="258"/>
@@ -14094,13 +14117,13 @@
       <c r="D53" s="273"/>
       <c r="E53" s="274"/>
       <c r="F53" s="275" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G53" s="276" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H53" s="277" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I53" s="278"/>
       <c r="J53" s="278"/>
@@ -14280,13 +14303,13 @@
       <c r="D54" s="273"/>
       <c r="E54" s="274"/>
       <c r="F54" s="275" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G54" s="279" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H54" s="277" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I54" s="278"/>
       <c r="J54" s="278"/>
@@ -14822,7 +14845,7 @@
       <c r="D57" s="255"/>
       <c r="E57" s="256"/>
       <c r="F57" s="265" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G57" s="257"/>
       <c r="H57" s="258"/>
@@ -15004,10 +15027,10 @@
       <c r="D58" s="163"/>
       <c r="E58" s="164"/>
       <c r="F58" s="219" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G58" s="231" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H58" s="232"/>
       <c r="I58" s="166"/>
@@ -15368,7 +15391,7 @@
       <c r="D60" s="255"/>
       <c r="E60" s="256"/>
       <c r="F60" s="265" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G60" s="257"/>
       <c r="H60" s="258"/>
@@ -15550,13 +15573,13 @@
       <c r="D61" s="163"/>
       <c r="E61" s="164"/>
       <c r="F61" s="219" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G61" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H61" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I61" s="166"/>
       <c r="J61" s="166"/>
@@ -15567,8 +15590,8 @@
       <c r="O61" s="169">
         <v>1</v>
       </c>
-      <c r="P61" s="301" t="s">
-        <v>302</v>
+      <c r="P61" s="304" t="s">
+        <v>297</v>
       </c>
       <c r="Q61" s="130"/>
       <c r="R61" s="131" t="str">
@@ -15740,13 +15763,13 @@
       <c r="D62" s="163"/>
       <c r="E62" s="164"/>
       <c r="F62" s="219" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G62" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H62" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I62" s="166"/>
       <c r="J62" s="166"/>
@@ -15757,7 +15780,7 @@
       <c r="O62" s="169">
         <v>1</v>
       </c>
-      <c r="P62" s="302"/>
+      <c r="P62" s="305"/>
       <c r="Q62" s="130"/>
       <c r="R62" s="131" t="str">
         <f>IF($J62="","",IF($J62&lt;=$L$2,$K62,IF($I62&lt;=$L$2,NETWORKDAYS($I62,$L$2,holiday!$C$3:$C$10)/NETWORKDAYS($I62,$J62,holiday!$C$3:$C$10)*$K62,0)))</f>
@@ -15928,13 +15951,13 @@
       <c r="D63" s="163"/>
       <c r="E63" s="164"/>
       <c r="F63" s="219" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G63" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H63" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I63" s="166"/>
       <c r="J63" s="166"/>
@@ -15945,7 +15968,7 @@
       <c r="O63" s="169">
         <v>1</v>
       </c>
-      <c r="P63" s="302"/>
+      <c r="P63" s="305"/>
       <c r="Q63" s="130"/>
       <c r="R63" s="131" t="str">
         <f>IF($J63="","",IF($J63&lt;=$L$2,$K63,IF($I63&lt;=$L$2,NETWORKDAYS($I63,$L$2,holiday!$C$3:$C$10)/NETWORKDAYS($I63,$J63,holiday!$C$3:$C$10)*$K63,0)))</f>
@@ -16116,13 +16139,13 @@
       <c r="D64" s="163"/>
       <c r="E64" s="164"/>
       <c r="F64" s="219" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G64" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H64" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I64" s="166"/>
       <c r="J64" s="166"/>
@@ -16133,7 +16156,7 @@
       <c r="O64" s="169">
         <v>1</v>
       </c>
-      <c r="P64" s="302"/>
+      <c r="P64" s="305"/>
       <c r="Q64" s="130"/>
       <c r="R64" s="131" t="str">
         <f>IF($J64="","",IF($J64&lt;=$L$2,$K64,IF($I64&lt;=$L$2,NETWORKDAYS($I64,$L$2,holiday!$C$3:$C$10)/NETWORKDAYS($I64,$J64,holiday!$C$3:$C$10)*$K64,0)))</f>
@@ -16304,13 +16327,13 @@
       <c r="D65" s="163"/>
       <c r="E65" s="164"/>
       <c r="F65" s="219" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G65" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H65" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I65" s="166"/>
       <c r="J65" s="166"/>
@@ -16321,7 +16344,7 @@
       <c r="O65" s="169">
         <v>1</v>
       </c>
-      <c r="P65" s="302"/>
+      <c r="P65" s="305"/>
       <c r="Q65" s="130"/>
       <c r="R65" s="131" t="str">
         <f>IF($J65="","",IF($J65&lt;=$L$2,$K65,IF($I65&lt;=$L$2,NETWORKDAYS($I65,$L$2,holiday!$C$3:$C$10)/NETWORKDAYS($I65,$J65,holiday!$C$3:$C$10)*$K65,0)))</f>
@@ -16492,13 +16515,13 @@
       <c r="D66" s="163"/>
       <c r="E66" s="164"/>
       <c r="F66" s="219" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G66" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H66" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I66" s="166"/>
       <c r="J66" s="166"/>
@@ -16509,7 +16532,7 @@
       <c r="O66" s="169">
         <v>1</v>
       </c>
-      <c r="P66" s="303"/>
+      <c r="P66" s="306"/>
       <c r="Q66" s="130"/>
       <c r="R66" s="131" t="str">
         <f>IF($J66="","",IF($J66&lt;=$L$2,$K66,IF($I66&lt;=$L$2,NETWORKDAYS($I66,$L$2,holiday!$C$3:$C$10)/NETWORKDAYS($I66,$J66,holiday!$C$3:$C$10)*$K66,0)))</f>
@@ -17036,7 +17059,7 @@
       <c r="D69" s="255"/>
       <c r="E69" s="256"/>
       <c r="F69" s="265" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G69" s="257"/>
       <c r="H69" s="258"/>
@@ -17218,10 +17241,10 @@
       <c r="D70" s="163"/>
       <c r="E70" s="164"/>
       <c r="F70" s="233" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G70" s="231" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H70" s="232"/>
       <c r="I70" s="166"/>
@@ -17234,7 +17257,7 @@
         <v>1</v>
       </c>
       <c r="P70" s="286" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="Q70" s="130"/>
       <c r="R70" s="131" t="str">
@@ -17584,7 +17607,7 @@
       <c r="D72" s="255"/>
       <c r="E72" s="256"/>
       <c r="F72" s="265" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G72" s="257"/>
       <c r="H72" s="258"/>
@@ -17766,17 +17789,17 @@
       <c r="D73" s="163"/>
       <c r="E73" s="164"/>
       <c r="F73" s="233" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G73" s="231" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H73" s="232"/>
       <c r="I73" s="166">
-        <v>43696</v>
+        <v>43699</v>
       </c>
       <c r="J73" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K73" s="167">
         <v>16</v>
@@ -17788,7 +17811,7 @@
         <v>0</v>
       </c>
       <c r="P73" s="286" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="Q73" s="130"/>
       <c r="R73" s="131">
@@ -18138,7 +18161,7 @@
       <c r="D75" s="255"/>
       <c r="E75" s="256"/>
       <c r="F75" s="265" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G75" s="257"/>
       <c r="H75" s="258"/>
@@ -18320,7 +18343,7 @@
       <c r="D76" s="273"/>
       <c r="E76" s="274"/>
       <c r="F76" s="280" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G76" s="279"/>
       <c r="H76" s="299"/>
@@ -18678,13 +18701,15 @@
       <c r="D78" s="243"/>
       <c r="E78" s="244"/>
       <c r="F78" s="245" t="s">
-        <v>181</v>
+        <v>309</v>
       </c>
       <c r="G78" s="246"/>
       <c r="H78" s="247"/>
       <c r="I78" s="248"/>
       <c r="J78" s="248"/>
-      <c r="K78" s="249"/>
+      <c r="K78" s="249">
+        <v>16</v>
+      </c>
       <c r="L78" s="250"/>
       <c r="M78" s="251"/>
       <c r="N78" s="252"/>
@@ -18858,7 +18883,7 @@
       <c r="D79" s="255"/>
       <c r="E79" s="256"/>
       <c r="F79" s="265" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G79" s="257"/>
       <c r="H79" s="258"/>
@@ -19040,13 +19065,13 @@
       <c r="D80" s="163"/>
       <c r="E80" s="164"/>
       <c r="F80" s="233" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G80" s="222" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H80" s="232" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I80" s="166"/>
       <c r="J80" s="166"/>
@@ -19056,7 +19081,7 @@
       <c r="N80" s="168"/>
       <c r="O80" s="169"/>
       <c r="P80" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q80" s="130"/>
       <c r="R80" s="131" t="str">
@@ -19228,13 +19253,13 @@
       <c r="D81" s="163"/>
       <c r="E81" s="164"/>
       <c r="F81" s="233" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G81" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H81" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I81" s="166"/>
       <c r="J81" s="166"/>
@@ -19244,7 +19269,7 @@
       <c r="N81" s="168"/>
       <c r="O81" s="169"/>
       <c r="P81" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q81" s="130"/>
       <c r="R81" s="131" t="str">
@@ -19416,13 +19441,13 @@
       <c r="D82" s="163"/>
       <c r="E82" s="164"/>
       <c r="F82" s="233" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G82" s="231" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H82" s="223" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I82" s="166"/>
       <c r="J82" s="166"/>
@@ -19432,7 +19457,7 @@
       <c r="N82" s="168"/>
       <c r="O82" s="169"/>
       <c r="P82" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q82" s="130"/>
       <c r="R82" s="131" t="str">
@@ -19604,19 +19629,19 @@
       <c r="D83" s="163"/>
       <c r="E83" s="164"/>
       <c r="F83" s="233" t="s">
-        <v>243</v>
+        <v>310</v>
       </c>
       <c r="G83" s="231" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H83" s="232" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I83" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="J83" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="K83" s="167">
         <v>2</v>
@@ -19626,7 +19651,7 @@
       <c r="N83" s="168"/>
       <c r="O83" s="169"/>
       <c r="P83" s="286" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="Q83" s="130"/>
       <c r="R83" s="131">
@@ -19798,13 +19823,13 @@
       <c r="D84" s="288"/>
       <c r="E84" s="289"/>
       <c r="F84" s="290" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G84" s="291" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H84" s="292" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I84" s="293"/>
       <c r="J84" s="293"/>
@@ -19814,7 +19839,7 @@
       <c r="N84" s="295"/>
       <c r="O84" s="296"/>
       <c r="P84" s="286" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="Q84" s="130"/>
       <c r="R84" s="131" t="str">
@@ -19986,13 +20011,13 @@
       <c r="D85" s="163"/>
       <c r="E85" s="164"/>
       <c r="F85" s="233" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G85" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H85" s="232" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I85" s="166"/>
       <c r="J85" s="166"/>
@@ -20002,7 +20027,7 @@
       <c r="N85" s="168"/>
       <c r="O85" s="169"/>
       <c r="P85" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q85" s="130"/>
       <c r="R85" s="131" t="str">
@@ -20174,13 +20199,13 @@
       <c r="D86" s="163"/>
       <c r="E86" s="164"/>
       <c r="F86" s="233" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G86" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H86" s="232" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I86" s="166"/>
       <c r="J86" s="166"/>
@@ -20190,7 +20215,7 @@
       <c r="N86" s="168"/>
       <c r="O86" s="169"/>
       <c r="P86" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q86" s="130"/>
       <c r="R86" s="131" t="str">
@@ -20362,13 +20387,13 @@
       <c r="D87" s="163"/>
       <c r="E87" s="164"/>
       <c r="F87" s="233" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="G87" s="231" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H87" s="232" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I87" s="166"/>
       <c r="J87" s="166"/>
@@ -20378,7 +20403,7 @@
       <c r="N87" s="168"/>
       <c r="O87" s="169"/>
       <c r="P87" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q87" s="130"/>
       <c r="R87" s="131" t="str">
@@ -20550,10 +20575,10 @@
       <c r="D88" s="163"/>
       <c r="E88" s="164"/>
       <c r="F88" s="233" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="G88" s="231" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H88" s="223"/>
       <c r="I88" s="166"/>
@@ -20564,7 +20589,7 @@
       <c r="N88" s="168"/>
       <c r="O88" s="169"/>
       <c r="P88" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q88" s="130"/>
       <c r="R88" s="131" t="str">
@@ -20736,13 +20761,13 @@
       <c r="D89" s="163"/>
       <c r="E89" s="164"/>
       <c r="F89" s="233" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="G89" s="222" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H89" s="223" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I89" s="166"/>
       <c r="J89" s="166"/>
@@ -20752,7 +20777,7 @@
       <c r="N89" s="168"/>
       <c r="O89" s="169"/>
       <c r="P89" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q89" s="130"/>
       <c r="R89" s="131" t="str">
@@ -20924,10 +20949,10 @@
       <c r="D90" s="163"/>
       <c r="E90" s="164"/>
       <c r="F90" s="233" t="s">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c r="G90" s="231" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H90" s="223"/>
       <c r="I90" s="166"/>
@@ -20938,7 +20963,7 @@
       <c r="N90" s="168"/>
       <c r="O90" s="169"/>
       <c r="P90" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q90" s="130"/>
       <c r="R90" s="131" t="str">
@@ -21120,7 +21145,7 @@
       <c r="N91" s="168"/>
       <c r="O91" s="169"/>
       <c r="P91" s="286" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="Q91" s="130"/>
       <c r="R91" s="131" t="str">
@@ -21290,7 +21315,7 @@
       <c r="D92" s="255"/>
       <c r="E92" s="256"/>
       <c r="F92" s="265" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G92" s="257"/>
       <c r="H92" s="258"/>
@@ -21472,19 +21497,19 @@
       <c r="D93" s="163"/>
       <c r="E93" s="164"/>
       <c r="F93" s="233" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="G93" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H93" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I93" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="J93" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="K93" s="167">
         <v>4</v>
@@ -21666,19 +21691,19 @@
       <c r="D94" s="163"/>
       <c r="E94" s="164"/>
       <c r="F94" s="219" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G94" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H94" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I94" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="J94" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="K94" s="167">
         <v>2</v>
@@ -21860,19 +21885,19 @@
       <c r="D95" s="163"/>
       <c r="E95" s="164"/>
       <c r="F95" s="219" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G95" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H95" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I95" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="J95" s="166">
-        <v>43693</v>
+        <v>43698</v>
       </c>
       <c r="K95" s="167">
         <v>2</v>
@@ -22054,19 +22079,19 @@
       <c r="D96" s="163"/>
       <c r="E96" s="164"/>
       <c r="F96" s="219" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G96" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H96" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I96" s="166">
-        <v>43696</v>
+        <v>43699</v>
       </c>
       <c r="J96" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K96" s="167">
         <v>1</v>
@@ -22248,19 +22273,19 @@
       <c r="D97" s="163"/>
       <c r="E97" s="164"/>
       <c r="F97" s="219" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G97" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H97" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I97" s="166">
-        <v>43696</v>
+        <v>43699</v>
       </c>
       <c r="J97" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K97" s="167">
         <v>1</v>
@@ -22334,19 +22359,19 @@
       <c r="D98" s="163"/>
       <c r="E98" s="164"/>
       <c r="F98" s="219" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G98" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H98" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I98" s="166">
-        <v>43696</v>
+        <v>43699</v>
       </c>
       <c r="J98" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K98" s="167">
         <v>2</v>
@@ -22528,19 +22553,19 @@
       <c r="D99" s="163"/>
       <c r="E99" s="164"/>
       <c r="F99" s="219" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G99" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H99" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I99" s="166">
-        <v>43696</v>
+        <v>43699</v>
       </c>
       <c r="J99" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K99" s="167">
         <v>1</v>
@@ -22722,19 +22747,19 @@
       <c r="D100" s="163"/>
       <c r="E100" s="164"/>
       <c r="F100" s="219" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G100" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H100" s="232" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I100" s="166">
-        <v>43696</v>
+        <v>43699</v>
       </c>
       <c r="J100" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K100" s="167">
         <v>1</v>
@@ -22916,13 +22941,13 @@
       <c r="D101" s="273"/>
       <c r="E101" s="274"/>
       <c r="F101" s="275" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G101" s="276" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H101" s="299" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I101" s="278"/>
       <c r="J101" s="278"/>
@@ -23280,7 +23305,7 @@
       <c r="D103" s="243"/>
       <c r="E103" s="244"/>
       <c r="F103" s="245" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G103" s="246"/>
       <c r="H103" s="247"/>
@@ -23460,19 +23485,19 @@
       <c r="D104" s="163"/>
       <c r="E104" s="164"/>
       <c r="F104" s="212" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G104" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H104" s="223" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I104" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="J104" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K104" s="167">
         <v>2</v>
@@ -23652,13 +23677,13 @@
       <c r="D105" s="163"/>
       <c r="E105" s="164"/>
       <c r="F105" s="285" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G105" s="222" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H105" s="223" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I105" s="166"/>
       <c r="J105" s="166"/>
@@ -24012,7 +24037,7 @@
       <c r="D107" s="243"/>
       <c r="E107" s="244"/>
       <c r="F107" s="245" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G107" s="246"/>
       <c r="H107" s="247"/>
@@ -24192,19 +24217,19 @@
       <c r="D108" s="163"/>
       <c r="E108" s="164"/>
       <c r="F108" s="285" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G108" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H108" s="223" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I108" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="J108" s="166">
-        <v>43697</v>
+        <v>43700</v>
       </c>
       <c r="K108" s="167">
         <v>2</v>
@@ -24384,19 +24409,19 @@
       <c r="D109" s="163"/>
       <c r="E109" s="164"/>
       <c r="F109" s="285" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G109" s="222" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H109" s="223" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I109" s="166">
-        <v>43698</v>
+        <v>43703</v>
       </c>
       <c r="J109" s="166">
-        <v>43698</v>
+        <v>43703</v>
       </c>
       <c r="K109" s="167">
         <v>4</v>
@@ -24928,7 +24953,7 @@
       <c r="H112" s="216"/>
       <c r="I112" s="166"/>
       <c r="J112" s="176" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K112" s="177" t="s">
         <v>154</v>
@@ -25102,11 +25127,11 @@
       <c r="I113" s="185"/>
       <c r="J113" s="185">
         <f>MAX(J6:J111)</f>
-        <v>43698</v>
+        <v>43703</v>
       </c>
       <c r="K113" s="186">
         <f>SUM(K6:K111)</f>
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="L113" s="187"/>
       <c r="M113" s="185">
@@ -25182,19 +25207,19 @@
       <c r="Q115" s="130"/>
       <c r="R115" s="143">
         <f>SUM(R6:R111)</f>
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="S115" s="143">
         <f>SUM(S6:S111)</f>
-        <v>0</v>
+        <v>6.9</v>
       </c>
       <c r="T115" s="143">
         <f>SUM(T6:T111)</f>
-        <v>0</v>
+        <v>6.9</v>
       </c>
       <c r="U115" s="143">
         <f>K113</f>
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="V115" s="130"/>
       <c r="W115" s="130"/>
@@ -25308,23 +25333,23 @@
       <c r="Q119" s="130"/>
       <c r="R119" s="143">
         <f>S115-R115</f>
-        <v>-39</v>
+        <v>-58.1</v>
       </c>
       <c r="S119" s="147">
         <f>S115-T115</f>
         <v>0</v>
       </c>
-      <c r="T119" s="148" t="e">
+      <c r="T119" s="148">
         <f>S115/T115</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="U119" s="148">
         <f>S115/R115</f>
-        <v>0</v>
+        <v>0.10615384615384615</v>
       </c>
       <c r="V119" s="143">
         <f>U115-S115</f>
-        <v>40</v>
+        <v>75.099999999999994</v>
       </c>
       <c r="W119" s="143" t="e">
         <f>T115+#REF!</f>
@@ -25488,48 +25513,48 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
-  <conditionalFormatting sqref="L7:L12 L16:L20 L24:L32 L34:L39 L42:L45 L47:L51 L53:L55 L58:L59 L61:L67 L70:L71 L73:L74 L76:L77 L80:L91 L93:L102 L104:L106 L108:L110 L22">
-    <cfRule type="expression" dxfId="8" priority="2196" stopIfTrue="1">
+  <conditionalFormatting sqref="L16:L20 L24:L32 L34:L39 L42:L45 L47:L51 L53:L55 L58:L59 L61:L67 L70:L71 L73:L74 L76:L77 L80:L91 L93:L102 L104:L106 L108:L110 L22 L7:L12">
+    <cfRule type="expression" dxfId="9" priority="2196" stopIfTrue="1">
       <formula>AND(($L7=""),AND(($I7&lt;&gt;""),($I7&lt;=$M$2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7:M12 M16:M20 M24:M32 M34:M39 M42:M45 M47:M51 M53:M55 M58:M59 M61:M67 M70:M71 M73:M74 M76:M77 M80:M91 M93:M102 M104:M106 M108:M110 M22">
-    <cfRule type="expression" dxfId="7" priority="2195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="2195" stopIfTrue="1">
       <formula>AND(($M7=""),AND(($J7&lt;&gt;""),($J7&lt;=$M$2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:O12 O16:O20 O24:O32 O34:O39 O42:O45 O47:O51 O53:O55 O58:O59 O61:O67 O70:O71 O73:O74 O76:O77 O80:O91 O104:O106 O108:O110 O93:O102 O22">
-    <cfRule type="expression" dxfId="6" priority="2193" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="2193" stopIfTrue="1">
       <formula>AND(($O7&lt;1),AND(($J7&lt;&gt;""),($J7&lt;$M$2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6:BG11">
-    <cfRule type="expression" dxfId="5" priority="230" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="230" stopIfTrue="1">
       <formula>AND(($I6&lt;&gt;""),AND(Y$4&gt;=$I6,Y$4&lt;=$J6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6:BG20 Y22:BG112">
-    <cfRule type="expression" dxfId="4" priority="228" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="228" stopIfTrue="1">
       <formula>OR(Y$5="六",Y$5="日")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>AND(($L21=""),AND(($I21&lt;&gt;""),($I21&lt;=$M$2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND(($M21=""),AND(($J21&lt;&gt;""),($J21&lt;=$M$2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O21">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>AND(($O21&lt;1),AND(($J21&lt;&gt;""),($J21&lt;$M$2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y21:BG21">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>OR(Y$5="六",Y$5="日")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25576,21 +25601,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="31" customFormat="1" ht="17.25" customHeight="1" thickTop="1">
-      <c r="A1" s="349" t="s">
+      <c r="A1" s="352" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="350"/>
-      <c r="C1" s="350"/>
-      <c r="D1" s="350"/>
-      <c r="E1" s="350"/>
-      <c r="F1" s="350"/>
-      <c r="G1" s="350"/>
-      <c r="H1" s="350"/>
-      <c r="I1" s="350"/>
-      <c r="J1" s="350"/>
-      <c r="K1" s="350"/>
-      <c r="L1" s="350"/>
-      <c r="M1" s="350"/>
+      <c r="B1" s="353"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="353"/>
+      <c r="F1" s="353"/>
+      <c r="G1" s="353"/>
+      <c r="H1" s="353"/>
+      <c r="I1" s="353"/>
+      <c r="J1" s="353"/>
+      <c r="K1" s="353"/>
+      <c r="L1" s="353"/>
+      <c r="M1" s="353"/>
       <c r="N1" s="12" t="s">
         <v>61</v>
       </c>
@@ -25606,22 +25631,22 @@
       <c r="R1" s="13"/>
       <c r="S1" s="14"/>
       <c r="T1" s="15"/>
-      <c r="U1" s="338"/>
+      <c r="U1" s="341"/>
     </row>
     <row r="2" spans="1:25" s="31" customFormat="1" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A2" s="351"/>
-      <c r="B2" s="352"/>
-      <c r="C2" s="352"/>
-      <c r="D2" s="352"/>
-      <c r="E2" s="352"/>
-      <c r="F2" s="352"/>
-      <c r="G2" s="352"/>
-      <c r="H2" s="352"/>
-      <c r="I2" s="352"/>
-      <c r="J2" s="352"/>
-      <c r="K2" s="352"/>
-      <c r="L2" s="352"/>
-      <c r="M2" s="352"/>
+      <c r="A2" s="354"/>
+      <c r="B2" s="355"/>
+      <c r="C2" s="355"/>
+      <c r="D2" s="355"/>
+      <c r="E2" s="355"/>
+      <c r="F2" s="355"/>
+      <c r="G2" s="355"/>
+      <c r="H2" s="355"/>
+      <c r="I2" s="355"/>
+      <c r="J2" s="355"/>
+      <c r="K2" s="355"/>
+      <c r="L2" s="355"/>
+      <c r="M2" s="355"/>
       <c r="N2" s="16" t="s">
         <v>18</v>
       </c>
@@ -25633,18 +25658,18 @@
       <c r="R2" s="19"/>
       <c r="S2" s="20"/>
       <c r="T2" s="21"/>
-      <c r="U2" s="339"/>
+      <c r="U2" s="342"/>
     </row>
     <row r="3" spans="1:25" ht="9.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="4" spans="1:25" ht="12.6" customHeight="1">
-      <c r="A4" s="353" t="s">
+      <c r="A4" s="356" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="354"/>
-      <c r="C4" s="354"/>
-      <c r="D4" s="355"/>
-      <c r="E4" s="355"/>
-      <c r="F4" s="358" t="s">
+      <c r="B4" s="357"/>
+      <c r="C4" s="357"/>
+      <c r="D4" s="358"/>
+      <c r="E4" s="358"/>
+      <c r="F4" s="361" t="s">
         <v>57</v>
       </c>
       <c r="G4" s="36" t="s">
@@ -25659,39 +25684,39 @@
       <c r="J4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="337" t="s">
+      <c r="K4" s="340" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="335" t="s">
+      <c r="L4" s="338" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="345" t="s">
+      <c r="M4" s="348" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="342" t="s">
+      <c r="N4" s="345" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="343"/>
-      <c r="P4" s="344"/>
-      <c r="Q4" s="342" t="s">
+      <c r="O4" s="346"/>
+      <c r="P4" s="347"/>
+      <c r="Q4" s="345" t="s">
         <v>66</v>
       </c>
-      <c r="R4" s="343"/>
-      <c r="S4" s="344"/>
-      <c r="T4" s="347" t="s">
+      <c r="R4" s="346"/>
+      <c r="S4" s="347"/>
+      <c r="T4" s="350" t="s">
         <v>70</v>
       </c>
-      <c r="U4" s="340" t="s">
+      <c r="U4" s="343" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="24.95" customHeight="1" thickBot="1">
-      <c r="A5" s="356"/>
-      <c r="B5" s="357"/>
-      <c r="C5" s="357"/>
-      <c r="D5" s="357"/>
-      <c r="E5" s="357"/>
-      <c r="F5" s="359"/>
+      <c r="A5" s="359"/>
+      <c r="B5" s="360"/>
+      <c r="C5" s="360"/>
+      <c r="D5" s="360"/>
+      <c r="E5" s="360"/>
+      <c r="F5" s="362"/>
       <c r="G5" s="35"/>
       <c r="H5" s="37" t="s">
         <v>26</v>
@@ -25702,9 +25727,9 @@
       <c r="J5" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="336"/>
-      <c r="L5" s="336"/>
-      <c r="M5" s="346"/>
+      <c r="K5" s="339"/>
+      <c r="L5" s="339"/>
+      <c r="M5" s="349"/>
       <c r="N5" s="22" t="s">
         <v>55</v>
       </c>
@@ -25723,8 +25748,8 @@
       <c r="S5" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="348"/>
-      <c r="U5" s="341"/>
+      <c r="T5" s="351"/>
+      <c r="U5" s="344"/>
       <c r="W5" s="32" t="s">
         <v>30</v>
       </c>
@@ -31205,13 +31230,13 @@
         <v>152</v>
       </c>
       <c r="C2" s="224" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="224" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="224" t="s">
         <v>214</v>
-      </c>
-      <c r="D2" s="224" t="s">
-        <v>213</v>
-      </c>
-      <c r="E2" s="224" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="2:5">
@@ -31222,7 +31247,7 @@
         <v>43623</v>
       </c>
       <c r="D3" s="226" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E3" s="228"/>
     </row>
@@ -31234,7 +31259,7 @@
         <v>43661</v>
       </c>
       <c r="D4" s="226" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E4" s="229"/>
     </row>

</xml_diff>